<commit_message>
Tweaked the dataset and updated the database connection
</commit_message>
<xml_diff>
--- a/food_carbon_footprint_2018.xlsx
+++ b/food_carbon_footprint_2018.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\data_science\portfolio_projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\data_science\portfolio_projects\food_carbon_fp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC38757C-8BF9-45B7-81E8-712875E51B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F59EF3F-B21C-4DA2-9B6D-C3567BBB25CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E02DE3BA-C597-40D5-9683-C5ED52DBDAFD}"/>
   </bookViews>
@@ -7499,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69759D-7ED9-4C82-9D3A-893D1D65AC30}">
   <dimension ref="A1:AA132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7554,7 +7554,7 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">

</xml_diff>